<commit_message>
final version hopefully, added graphs, model assumptions
</commit_message>
<xml_diff>
--- a/output/execution_times/execution_times_python.xlsx
+++ b/output/execution_times/execution_times_python.xlsx
@@ -10,6 +10,12 @@
     <sheet name="ANOVA_statsmodels" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="LR - Refactored" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="ANOVA - OOP" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ANOVA_scipy" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="LR_statsmodels" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ANOVA - own" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="LR_scipy" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="LR - OOP" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="LR_scikit" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,6 +538,81 @@
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ANOVA_statsmodels</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1.267473697662354</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-04-06 13:56:07</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ANOVA_statsmodels</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7016973495483398</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-04-06 13:56:50</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ANOVA_statsmodels</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6571199893951416</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-04-06 13:59:16</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Python</t>
         </is>
@@ -548,7 +629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,6 +709,156 @@
         </is>
       </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>LR - Refactored</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.872143030166626</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:12:13</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LR - Refactored</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8297958374023438</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:13:36</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LR - Refactored</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1.045719623565674</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:13:59</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LR - Refactored</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8370492458343506</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:14:25</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LR - Refactored</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8381400108337402</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:15:29</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>LR - Refactored</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8531451225280762</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:17:37</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>Python</t>
         </is>
@@ -732,4 +963,1005 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Method</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Execution_time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ANOVA_scipy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1.098573446273804</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:07:06</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Method</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Execution_time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.4333217144012451</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:33:49</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.4305281639099121</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:37:15</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.4194924831390381</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:37:42</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5031492710113525</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:45:55</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.506821870803833</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:50:32</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5210192203521729</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:51:25</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5268058776855469</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:52:58</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.519690990447998</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:54:24</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.5066597461700439</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-04-06 14:54:38</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.5097739696502686</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-04-06 16:53:19</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LR_statsmodels</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5095155239105225</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-04-06 16:54:33</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Method</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Execution_time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ANOVA - own</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3861253261566162</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:06:12</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ANOVA - own</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.3585975170135498</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:09:58</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ANOVA - own</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3415231704711914</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:11:30</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ANOVA - own</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3329277038574219</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:12:13</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ANOVA - own</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.3573248386383057</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:13:41</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ANOVA - own</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.4382288455963135</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-04-06 15:15:13</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Method</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Execution_time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LR_scipy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.5450637340545654</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-04-06 16:57:50</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>LR_scipy</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5122549533843994</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:05:49</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>LR_scipy</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5028741359710693</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:06:17</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LR_scipy</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5068609714508057</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:13:23</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LR_scipy</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5104579925537109</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:16:17</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LR_scipy</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5449540615081787</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:16:40</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LR_scipy</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5083544254302979</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:17:23</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Method</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Execution_time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LR - OOP</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.6794648170471191</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:22:07</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>LR - OOP</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.7250077724456787</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:22:32</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>LR - OOP</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.68916916847229</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:22:47</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Method</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Execution_time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LR_scikit</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Windows Ryzen 9 5900x 32GB</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.497309684753418</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-04-06 17:24:45</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>